<commit_message>
Add Text entry type support for lab calculators
- Add studentTextTrial1/2 fields to CalculationRow interface
- Implement setStudentText action in calculator store
- Update CSV parser to initialize text fields and handle Text entry type
- Add text input handling in CalculatorRow component
- Update CalculatorGrid and App to pass through text change handlers
- Support for text fields like 'Name of diprotic acid' in titration lab
</commit_message>
<xml_diff>
--- a/Excel Logic/KaKb Key Calculator Formulas.xlsx
+++ b/Excel Logic/KaKb Key Calculator Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkawagoe/Scripts/Lab Check/KaKb Lab/Excel Logic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4A6060D-75EB-F54B-9446-22BD4164DADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E5A077D1-55CB-CB4F-A32C-C05D255B5BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="36000" windowHeight="22580" xr2:uid="{A489C9C8-2BC1-984E-9DE9-D2012CFE6641}"/>
   </bookViews>
@@ -452,12 +452,6 @@
     <t>G58</t>
   </si>
   <si>
-    <t>Trial 1 Data Tag</t>
-  </si>
-  <si>
-    <t>Trial 2 Data Tag</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
@@ -477,6 +471,12 @@
   </si>
   <si>
     <t>Tolerance 2</t>
+  </si>
+  <si>
+    <t>DataRef1</t>
+  </si>
+  <si>
+    <t>DataRef2</t>
   </si>
 </sst>
 </file>
@@ -907,7 +907,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,19 +919,19 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" t="s">
         <v>143</v>
-      </c>
-      <c r="B1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C1" t="s">
-        <v>145</v>
       </c>
       <c r="D1" s="8">
         <v>0.1</v>
       </c>
       <c r="E1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F1" s="8">
         <v>0.15</v>
@@ -945,10 +945,10 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="E2" t="s">
         <v>47</v>
@@ -1387,7 +1387,7 @@
         <v>2.9120158626775136E-5</v>
       </c>
       <c r="G23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H23" t="s">
         <v>28</v>
@@ -1411,7 +1411,7 @@
         <v>-0.65455446743040535</v>
       </c>
       <c r="G24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H24" t="s">
         <v>29</v>
@@ -1441,7 +1441,7 @@
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G27" s="1">
         <v>1</v>
@@ -1845,7 +1845,7 @@
         <v>1.8637790035011686E-5</v>
       </c>
       <c r="G45" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H45" t="s">
         <v>28</v>
@@ -2115,10 +2115,10 @@
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D59" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E59" t="s">
         <v>19</v>
@@ -2128,7 +2128,7 @@
         <v>9.1347834731286396E-6</v>
       </c>
       <c r="G59" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H59" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Fix calculation issues and add debugging features
- Fix CSV parsing for Colligative Properties calculator
- Update parser to recognize 'Sample' columns in addition to 'Trial' columns
- Fix cell reference replacement bug in formula engine (F40 vs F4 conflict)
- Add comprehensive debugging logging for formula calculations
- Fix TypeScript error in CalculatorSelector component
- Add temporary logging to show expected values and calculation process
</commit_message>
<xml_diff>
--- a/Excel Logic/KaKb Key Calculator Formulas.xlsx
+++ b/Excel Logic/KaKb Key Calculator Formulas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jkawagoe/Scripts/Lab Check/KaKb Lab/Excel Logic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E5A077D1-55CB-CB4F-A32C-C05D255B5BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8D4FEAA-8DE7-A44D-8F34-A1E08645C2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="800" windowWidth="36000" windowHeight="22580" xr2:uid="{A489C9C8-2BC1-984E-9DE9-D2012CFE6641}"/>
   </bookViews>
@@ -907,7 +907,7 @@
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>